<commit_message>
Fix: Get all info from XML
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Månadsrapport för uppdragstagare LSS</t>
+  </si>
+  <si>
+    <t>PercentToAcceptFuzzy</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2854,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2961,7 +2964,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Before changing to dictionary instead of tables for procapita
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -204,9 +204,6 @@
     <t>PercentToAcceptFuzzy</t>
   </si>
   <si>
-    <t>OePUrl</t>
-  </si>
-  <si>
     <t>FlowInstance</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>FolderPathToReportedHours</t>
+  </si>
+  <si>
+    <t>ProcapitaRole</t>
   </si>
 </sst>
 </file>
@@ -2873,10 +2873,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3000,34 +3000,34 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
-        <v>61</v>
+      <c r="B13" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4013,7 +4013,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extracted all except for insaterna.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -213,13 +213,13 @@
     <t>FilePathToUtanordningslistaPDF</t>
   </si>
   <si>
-    <t>FilePathToExcelFileMoneyChartSF</t>
-  </si>
-  <si>
     <t>FolderPathToReportedHours</t>
   </si>
   <si>
     <t>ProcapitaRole</t>
+  </si>
+  <si>
+    <t>MaximumPrivateExpense</t>
   </si>
 </sst>
 </file>
@@ -2876,7 +2876,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3000,10 +3000,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3016,18 +3016,18 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Added function for saving receipts.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -182,13 +182,6 @@
     <t>Cred_NA_OeP</t>
   </si>
   <si>
-    <t xml:space="preserve">Cred_NA_Behorighetshantering_Berit
-</t>
-  </si>
-  <si>
-    <t>URLBerit</t>
-  </si>
-  <si>
     <t>OePHämtaStatus</t>
   </si>
   <si>
@@ -220,6 +213,15 @@
   </si>
   <si>
     <t>MaximumPrivateExpense</t>
+  </si>
+  <si>
+    <t>OePHämtaStatusArvoderadeUppdrag</t>
+  </si>
+  <si>
+    <t>FolderPathToCopies</t>
+  </si>
+  <si>
+    <t>FolderPathToReceipt</t>
   </si>
 </sst>
 </file>
@@ -599,7 +601,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -649,7 +651,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -692,12 +694,8 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2873,10 +2871,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2952,85 +2950,92 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>53</v>
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
+      <c r="A7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>55</v>
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4012,7 +4017,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: updated lib and screenshots.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>ExScreenshotsFolderPath</t>
   </si>
   <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -222,13 +216,22 @@
   </si>
   <si>
     <t>FolderPathToReceipt</t>
+  </si>
+  <si>
+    <t>\\safs008\RPA\VoF\RPA_030\Temp</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Arvoderade Uppdrag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -253,6 +256,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,10 +280,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -284,8 +294,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -648,49 +660,49 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1699,7 +1711,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1752,29 +1764,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="36" customHeight="1">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1782,113 +1794,113 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="45">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2864,8 +2876,11 @@
     <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2873,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2893,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2923,117 +2938,117 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Added screenshot for init app and number of retries.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1710,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1783,7 +1783,7 @@
         <v>44</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Fix: Handles assigning dates in december. Throws if no table from Procapita is found.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -192,12 +192,6 @@
   </si>
   <si>
     <t>FlowInstance</t>
-  </si>
-  <si>
-    <t>UtanordningslistaAsPDF</t>
-  </si>
-  <si>
-    <t>FilePathToUtanordningslistaPDF</t>
   </si>
   <si>
     <t>FolderPathToReportedHours</t>
@@ -683,7 +677,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1710,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1795,7 +1789,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1897,7 +1891,7 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>40</v>
@@ -2886,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2976,7 +2970,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3005,52 +2999,45 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>62</v>
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4031,7 +4018,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: Correct check if ok nr of month since report.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Arvoderade Uppdrag</t>
+  </si>
+  <si>
+    <t>OkNrOfMonthBack</t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1705,7 +1708,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1766,7 +1769,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -2883,7 +2886,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3037,7 +3040,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>